<commit_message>
hasta el 10 de abril
</commit_message>
<xml_diff>
--- a/2022.xlsx
+++ b/2022.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>2,37382</t>
   </si>
@@ -30,6 +30,9 @@
     <t>2,37717</t>
   </si>
   <si>
+    <t>2,37851</t>
+  </si>
+  <si>
     <t>2,37388</t>
   </si>
   <si>
@@ -39,6 +42,9 @@
     <t>2,37722</t>
   </si>
   <si>
+    <t>2,37856</t>
+  </si>
+  <si>
     <t>2,37394</t>
   </si>
   <si>
@@ -48,6 +54,9 @@
     <t>2,37727</t>
   </si>
   <si>
+    <t>2,37861</t>
+  </si>
+  <si>
     <t>2,37400</t>
   </si>
   <si>
@@ -57,6 +66,9 @@
     <t>2,37732</t>
   </si>
   <si>
+    <t>2,37866</t>
+  </si>
+  <si>
     <t>2,37406</t>
   </si>
   <si>
@@ -66,6 +78,9 @@
     <t>2,37737</t>
   </si>
   <si>
+    <t>2,37871</t>
+  </si>
+  <si>
     <t>2,37412</t>
   </si>
   <si>
@@ -75,6 +90,9 @@
     <t>2,37742</t>
   </si>
   <si>
+    <t>2,37876</t>
+  </si>
+  <si>
     <t>2,37418</t>
   </si>
   <si>
@@ -84,6 +102,9 @@
     <t>2,37747</t>
   </si>
   <si>
+    <t>2,37881</t>
+  </si>
+  <si>
     <t>2,37424</t>
   </si>
   <si>
@@ -93,6 +114,9 @@
     <t>2,37752</t>
   </si>
   <si>
+    <t>2,37886</t>
+  </si>
+  <si>
     <t>2,37430</t>
   </si>
   <si>
@@ -102,6 +126,9 @@
     <t>2,37757</t>
   </si>
   <si>
+    <t>2,37891</t>
+  </si>
+  <si>
     <t>2,37436</t>
   </si>
   <si>
@@ -111,121 +138,187 @@
     <t>2,37762</t>
   </si>
   <si>
+    <t>2,37896</t>
+  </si>
+  <si>
     <t>2,37442</t>
   </si>
   <si>
     <t>2,37627</t>
   </si>
   <si>
+    <t>2,37766</t>
+  </si>
+  <si>
     <t>2,37448</t>
   </si>
   <si>
     <t>2,37632</t>
   </si>
   <si>
+    <t>2,37770</t>
+  </si>
+  <si>
     <t>2,37454</t>
   </si>
   <si>
     <t>2,37637</t>
   </si>
   <si>
+    <t>2,37774</t>
+  </si>
+  <si>
     <t>2,37460</t>
   </si>
   <si>
     <t>2,37642</t>
   </si>
   <si>
+    <t>2,37778</t>
+  </si>
+  <si>
     <t>2,37466</t>
   </si>
   <si>
     <t>2,37647</t>
   </si>
   <si>
+    <t>2,37782</t>
+  </si>
+  <si>
     <t>2,37472</t>
   </si>
   <si>
     <t>2,37652</t>
   </si>
   <si>
+    <t>2,37786</t>
+  </si>
+  <si>
     <t>2,37478</t>
   </si>
   <si>
     <t>2,37657</t>
   </si>
   <si>
+    <t>2,37790</t>
+  </si>
+  <si>
     <t>2,37484</t>
   </si>
   <si>
     <t>2,37662</t>
   </si>
   <si>
+    <t>2,37794</t>
+  </si>
+  <si>
     <t>2,37490</t>
   </si>
   <si>
     <t>2,37667</t>
   </si>
   <si>
+    <t>2,37798</t>
+  </si>
+  <si>
     <t>2,37496</t>
   </si>
   <si>
     <t>2,37672</t>
   </si>
   <si>
+    <t>2,37802</t>
+  </si>
+  <si>
     <t>2,37502</t>
   </si>
   <si>
     <t>2,37677</t>
   </si>
   <si>
+    <t>2,37806</t>
+  </si>
+  <si>
     <t>2,37508</t>
   </si>
   <si>
     <t>2,37682</t>
   </si>
   <si>
+    <t>2,37810</t>
+  </si>
+  <si>
     <t>2,37514</t>
   </si>
   <si>
     <t>2,37687</t>
   </si>
   <si>
+    <t>2,37814</t>
+  </si>
+  <si>
     <t>2,37520</t>
   </si>
   <si>
     <t>2,37692</t>
   </si>
   <si>
+    <t>2,37818</t>
+  </si>
+  <si>
     <t>2,37526</t>
   </si>
   <si>
     <t>2,37697</t>
   </si>
   <si>
+    <t>2,37822</t>
+  </si>
+  <si>
     <t>2,37532</t>
   </si>
   <si>
     <t>2,37702</t>
   </si>
   <si>
+    <t>2,37826</t>
+  </si>
+  <si>
     <t>2,37538</t>
   </si>
   <si>
     <t>2,37707</t>
   </si>
   <si>
+    <t>2,37830</t>
+  </si>
+  <si>
     <t>2,37544</t>
   </si>
   <si>
     <t>2,37712</t>
   </si>
   <si>
+    <t>2,37834</t>
+  </si>
+  <si>
     <t>2,37550</t>
   </si>
   <si>
+    <t>2,37838</t>
+  </si>
+  <si>
     <t>2,37556</t>
   </si>
   <si>
+    <t>2,37842</t>
+  </si>
+  <si>
     <t>2,37562</t>
+  </si>
+  <si>
+    <t>2,37846</t>
   </si>
 </sst>
 </file>
@@ -642,7 +735,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,7 +753,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -672,15 +767,17 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -692,15 +789,17 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -712,15 +811,17 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -732,15 +833,17 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -752,15 +855,17 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -772,15 +877,17 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -792,15 +899,17 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -812,15 +921,17 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -832,15 +943,17 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -852,12 +965,14 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -870,12 +985,14 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -888,12 +1005,14 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -906,12 +1025,14 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -924,12 +1045,14 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -942,12 +1065,14 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -960,12 +1085,14 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -978,12 +1105,14 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -996,12 +1125,14 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1014,12 +1145,14 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1032,12 +1165,14 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1050,12 +1185,14 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1068,12 +1205,14 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1086,12 +1225,14 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1104,12 +1245,14 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1122,12 +1265,14 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1140,12 +1285,14 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1158,12 +1305,14 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1176,10 +1325,12 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1192,10 +1343,12 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1208,10 +1361,12 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>

</xml_diff>